<commit_message>
Rettet noget figur halløj, og lydstyrke og rettet i gestikker
</commit_message>
<xml_diff>
--- a/Content/Bilag/ElektroniskBilag/DataSocialAccept/Test2.xlsx
+++ b/Content/Bilag/ElektroniskBilag/DataSocialAccept/Test2.xlsx
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -65,12 +65,6 @@
     <t>Vært 6</t>
   </si>
   <si>
-    <t>Gengiver gestikken rigtigt</t>
-  </si>
-  <si>
-    <t>Gengiver gestikken delvist rigtigt</t>
-  </si>
-  <si>
     <t>Gengiver ikke gestikken</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t>Skru op</t>
+  </si>
+  <si>
+    <t>Gengiver gestikken delvist korrekt</t>
+  </si>
+  <si>
+    <t>Gengiver gestikken korrekt</t>
   </si>
 </sst>
 </file>
@@ -237,7 +237,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gengiver gestikken rigtigt</c:v>
+                  <c:v>Gengiver gestikken korrekt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -322,7 +322,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gengiver gestikken delvist rigtigt</c:v>
+                  <c:v>Gengiver gestikken delvist korrekt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3007,7 +3007,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3067,7 +3067,7 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J2">
         <v>4</v>
@@ -3105,7 +3105,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -3143,7 +3143,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0</v>

</xml_diff>